<commit_message>
Support the new match flow
</commit_message>
<xml_diff>
--- a/scenarios/cough/processes/PrevMed.xlsx
+++ b/scenarios/cough/processes/PrevMed.xlsx
@@ -390,6 +390,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">category = TO_TEXT(SELECT a.CategoryPrevMed FROM Products p JOIN API a ON p.APIID == a.ID WHERE p.ID == [</t>
     </r>
@@ -399,6 +400,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">PrevProduct</t>
     </r>
@@ -407,6 +409,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">]), </t>
     </r>
@@ -469,7 +472,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -534,17 +537,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -838,11 +830,11 @@
   </sheetPr>
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.38671875" defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.39453125" defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="19.7"/>

</xml_diff>

<commit_message>
Shorten the path to get to brand selection
</commit_message>
<xml_diff>
--- a/scenarios/cough/processes/PrevMed.xlsx
+++ b/scenarios/cough/processes/PrevMed.xlsx
@@ -25,7 +25,7 @@
     <author> </author>
   </authors>
   <commentList>
-    <comment ref="B11" authorId="0">
+    <comment ref="B7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +44,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D13" authorId="0">
+    <comment ref="D9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="83">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -122,33 +122,12 @@
     <t xml:space="preserve">Medication</t>
   </si>
   <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wie hieß denn das Medikament Dass du eingenommen hast?</t>
   </si>
   <si>
-    <t xml:space="preserve">Freitext-Eingabe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO(prev_brand)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Der genaue Name fällt mir leider gerade nicht ein. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO(prev_brand_no)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prev_brand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medication - Brand</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ups. Da hat leider was nicht funktioniert. Lass uns mal zusammen danach suchen. Von welcher der folgenden Marken war dein Hustenmedikament?</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO(prev_final)</t>
   </si>
   <si>
@@ -156,12 +135,6 @@
   </si>
   <si>
     <t xml:space="preserve">[PrevBrand]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prev_brand_no</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lass uns mal zusammen danach suchen. Von welcher der folgenden Marken war dein Hustenmedikament?</t>
   </si>
   <si>
     <t xml:space="preserve">prev_final</t>
@@ -520,13 +493,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFBFBFBF"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -534,6 +500,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -637,7 +610,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -690,56 +663,40 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -828,10 +785,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.39453125" defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -909,7 +866,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>16</v>
       </c>
@@ -917,327 +874,321 @@
         <v>17</v>
       </c>
       <c r="C5" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>29</v>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="E10" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="0" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="E11" s="10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B12" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="10" t="s">
+      <c r="E12" s="6"/>
+      <c r="G12" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G13" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="7" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>45</v>
+        <v>15</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+      <c r="A15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="11" t="s">
+      <c r="B15" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="G16" s="0" t="s">
+      <c r="E15" s="6"/>
+      <c r="G15" s="0" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>52</v>
+        <v>53</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="F20" s="18"/>
+    </row>
+    <row r="21" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" s="19"/>
+    </row>
+    <row r="22" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E22" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="G19" s="0" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="G20" s="19" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E22" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="43.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="D23" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="E23" s="22" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E23" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="145.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="11" t="s">
         <v>74</v>
       </c>
+      <c r="B24" s="11"/>
       <c r="C24" s="12" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="E24" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" s="23"/>
-    </row>
-    <row r="25" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E24" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
         <v>76</v>
       </c>
@@ -1247,107 +1198,53 @@
       <c r="C25" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E25" s="24"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="4"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="6" t="s">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E26" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="102" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="4" t="s">
+      <c r="E26" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="11"/>
-      <c r="C27" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D27" s="6" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="10" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="145.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="E28" s="25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="29.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="7"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="4"/>
-      <c r="B32" s="26"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7"/>
-      <c r="B33" s="27"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-    </row>
+    <row r="28" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="4"/>
+      <c r="B28" s="22"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+    </row>
+    <row r="29" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7"/>
+      <c r="B29" s="23"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>